<commit_message>
More work on legislation spreadsheet
</commit_message>
<xml_diff>
--- a/lists/legislation/port-health-authority.xlsx
+++ b/lists/legislation/port-health-authority.xlsx
@@ -293,7 +293,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -336,7 +336,7 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>

</xml_diff>